<commit_message>
text zum teilziel 2
</commit_message>
<xml_diff>
--- a/Vokabeln.xlsx
+++ b/Vokabeln.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felicitas\Documents\Studium\Medida\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54277187-88D5-42B3-B11F-14C0CC9A06A3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BE7A99-7DB3-42A4-9DFA-692EC235B780}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{C1AD5172-CF1A-4761-BB6C-B46EFA6E135A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="221">
   <si>
     <t xml:space="preserve">Deutsch </t>
   </si>
@@ -604,6 +604,90 @@
   </si>
   <si>
     <t>eagle</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>dolphin</t>
+  </si>
+  <si>
+    <t>Delfin</t>
+  </si>
+  <si>
+    <t>Pinguin</t>
+  </si>
+  <si>
+    <t>penguin</t>
+  </si>
+  <si>
+    <t>Maus</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>Kuh</t>
+  </si>
+  <si>
+    <t>cow</t>
+  </si>
+  <si>
+    <t>Ratte</t>
+  </si>
+  <si>
+    <t>rat</t>
+  </si>
+  <si>
+    <t>Schaf</t>
+  </si>
+  <si>
+    <t>sheep</t>
+  </si>
+  <si>
+    <t>Ente</t>
+  </si>
+  <si>
+    <t>duck</t>
+  </si>
+  <si>
+    <t>Gans</t>
+  </si>
+  <si>
+    <t>goose</t>
+  </si>
+  <si>
+    <t>Teppich</t>
+  </si>
+  <si>
+    <t>carpet</t>
+  </si>
+  <si>
+    <t>Badewanne</t>
+  </si>
+  <si>
+    <t>bathtub</t>
+  </si>
+  <si>
+    <t>Regal</t>
+  </si>
+  <si>
+    <t>Pullover</t>
+  </si>
+  <si>
+    <t>pullover</t>
+  </si>
+  <si>
+    <t>Mantel</t>
+  </si>
+  <si>
+    <t>coat</t>
+  </si>
+  <si>
+    <t>shelf</t>
   </si>
 </sst>
 </file>
@@ -957,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86941496-EC73-4429-B300-EA09A89D55C9}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1553,6 +1637,12 @@
       <c r="G30" t="s">
         <v>178</v>
       </c>
+      <c r="J30" t="s">
+        <v>193</v>
+      </c>
+      <c r="K30" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
@@ -1561,6 +1651,18 @@
       <c r="C31" t="s">
         <v>117</v>
       </c>
+      <c r="F31" t="s">
+        <v>211</v>
+      </c>
+      <c r="G31" t="s">
+        <v>212</v>
+      </c>
+      <c r="J31" t="s">
+        <v>196</v>
+      </c>
+      <c r="K31" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
@@ -1569,56 +1671,122 @@
       <c r="C32" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>213</v>
+      </c>
+      <c r="G32" t="s">
+        <v>214</v>
+      </c>
+      <c r="J32" t="s">
+        <v>197</v>
+      </c>
+      <c r="K32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>120</v>
       </c>
       <c r="C33" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>215</v>
+      </c>
+      <c r="G33" t="s">
+        <v>220</v>
+      </c>
+      <c r="J33" t="s">
+        <v>199</v>
+      </c>
+      <c r="K33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>122</v>
       </c>
       <c r="C34" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>216</v>
+      </c>
+      <c r="G34" t="s">
+        <v>217</v>
+      </c>
+      <c r="J34" t="s">
+        <v>201</v>
+      </c>
+      <c r="K34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>124</v>
       </c>
       <c r="C35" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>218</v>
+      </c>
+      <c r="G35" t="s">
+        <v>219</v>
+      </c>
+      <c r="J35" t="s">
+        <v>203</v>
+      </c>
+      <c r="K35" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>127</v>
       </c>
       <c r="C36" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="J36" t="s">
+        <v>205</v>
+      </c>
+      <c r="K36" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>128</v>
       </c>
       <c r="C37" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="J37" t="s">
+        <v>207</v>
+      </c>
+      <c r="K37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>129</v>
       </c>
       <c r="C38" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="J38" t="s">
+        <v>209</v>
+      </c>
+      <c r="K38" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>132</v>
       </c>
@@ -1626,7 +1794,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>134</v>
       </c>
@@ -1634,7 +1802,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Text Teilziel 2 and Vokabeln modified
</commit_message>
<xml_diff>
--- a/Vokabeln.xlsx
+++ b/Vokabeln.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felicitas\Documents\Studium\Medida\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BE7A99-7DB3-42A4-9DFA-692EC235B780}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EB5BD1-E3FE-4EDC-91DF-9C7D5A0AA610}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{C1AD5172-CF1A-4761-BB6C-B46EFA6E135A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="216">
   <si>
     <t xml:space="preserve">Deutsch </t>
   </si>
@@ -282,27 +282,6 @@
     <t>spicy</t>
   </si>
   <si>
-    <t>süß</t>
-  </si>
-  <si>
-    <t>sweet</t>
-  </si>
-  <si>
-    <t>salty</t>
-  </si>
-  <si>
-    <t>salzig</t>
-  </si>
-  <si>
-    <t>bitter</t>
-  </si>
-  <si>
-    <t>fettig</t>
-  </si>
-  <si>
-    <t>greasy</t>
-  </si>
-  <si>
     <t>Rock</t>
   </si>
   <si>
@@ -688,6 +667,12 @@
   </si>
   <si>
     <t>shelf</t>
+  </si>
+  <si>
+    <t>Saft</t>
+  </si>
+  <si>
+    <t>juice</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86941496-EC73-4429-B300-EA09A89D55C9}">
-  <dimension ref="A2:K41"/>
+  <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,10 +1083,10 @@
         <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="K3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1118,10 +1103,10 @@
         <v>62</v>
       </c>
       <c r="J4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1138,10 +1123,10 @@
         <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="K5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1158,10 +1143,10 @@
         <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="K6" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1178,10 +1163,10 @@
         <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1198,10 +1183,10 @@
         <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1218,10 +1203,10 @@
         <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="K9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1238,10 +1223,10 @@
         <v>71</v>
       </c>
       <c r="J10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="K10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1258,10 +1243,10 @@
         <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1278,10 +1263,10 @@
         <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K12" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1298,10 +1283,10 @@
         <v>68</v>
       </c>
       <c r="J13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="K13" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1318,10 +1303,10 @@
         <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K14" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1338,10 +1323,10 @@
         <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="K15" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1358,10 +1343,10 @@
         <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.35">
@@ -1378,10 +1363,10 @@
         <v>80</v>
       </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="K17" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
@@ -1392,16 +1377,16 @@
         <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="K18" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
@@ -1412,16 +1397,16 @@
         <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K19" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
@@ -1432,16 +1417,16 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
         <v>94</v>
       </c>
-      <c r="G20" t="s">
-        <v>101</v>
-      </c>
       <c r="J20" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K20" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
@@ -1452,16 +1437,16 @@
         <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="K21" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
@@ -1472,16 +1457,16 @@
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J22" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K22" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
@@ -1492,16 +1477,16 @@
         <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
@@ -1512,16 +1497,16 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K24" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
@@ -1532,16 +1517,16 @@
         <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G25" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="J25" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K25" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
@@ -1552,262 +1537,238 @@
         <v>84</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J26" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="K26" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>85</v>
+        <v>214</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>215</v>
       </c>
       <c r="F27" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="J27" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K27" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G28" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="K28" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J29" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K29" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G30" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J30" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="K30" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F31" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G31" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="J31" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="K31" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="J32" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="K32" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G33" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="J33" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K33" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F34" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G34" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="J34" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K34" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F35" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G35" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="J35" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="K35" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J36" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="K36" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="J37" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K37" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J38" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="K38" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>136</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
änderung vokabelliste (planked - blanket) & dateinamen geändert
</commit_message>
<xml_diff>
--- a/Vokabeln.xlsx
+++ b/Vokabeln.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Verri_Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Medida-JungleParty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C9A814-AFF2-4C4B-9B54-D95D59C3F6CC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DACBB7-C689-4CE5-8476-816708FBB7A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1AD5172-CF1A-4761-BB6C-B46EFA6E135A}"/>
   </bookViews>
@@ -231,9 +231,6 @@
     <t>bed sheet</t>
   </si>
   <si>
-    <t>planket</t>
-  </si>
-  <si>
     <t>couch</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>strawberry</t>
+  </si>
+  <si>
+    <t>blanket</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86941496-EC73-4429-B300-EA09A89D55C9}">
   <dimension ref="A2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,10 +1128,10 @@
         <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1148,10 +1148,10 @@
         <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1168,10 +1168,10 @@
         <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1188,10 +1188,10 @@
         <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1208,10 +1208,10 @@
         <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1228,10 +1228,10 @@
         <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1245,13 +1245,13 @@
         <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1265,13 +1265,13 @@
         <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>220</v>
       </c>
       <c r="J10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1288,10 +1288,10 @@
         <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1308,10 +1308,10 @@
         <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1328,10 +1328,10 @@
         <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1342,16 +1342,16 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
         <v>70</v>
       </c>
-      <c r="G14" t="s">
-        <v>71</v>
-      </c>
       <c r="J14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1362,16 +1362,16 @@
         <v>30</v>
       </c>
       <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
       <c r="J15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1382,16 +1382,16 @@
         <v>31</v>
       </c>
       <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" t="s">
         <v>74</v>
       </c>
-      <c r="G16" t="s">
-        <v>75</v>
-      </c>
       <c r="J16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1399,19 +1399,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
         <v>76</v>
       </c>
-      <c r="G17" t="s">
-        <v>77</v>
-      </c>
       <c r="J17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1422,16 +1422,16 @@
         <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1442,16 +1442,16 @@
         <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1462,16 +1462,16 @@
         <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1482,16 +1482,16 @@
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1502,16 +1502,16 @@
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J22" t="s">
+        <v>161</v>
+      </c>
+      <c r="K22" t="s">
         <v>162</v>
-      </c>
-      <c r="K22" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1522,96 +1522,96 @@
         <v>41</v>
       </c>
       <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
         <v>85</v>
       </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
       <c r="J23" t="s">
+        <v>166</v>
+      </c>
+      <c r="K23" t="s">
         <v>167</v>
-      </c>
-      <c r="K23" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" t="s">
         <v>92</v>
       </c>
-      <c r="G24" t="s">
-        <v>93</v>
-      </c>
       <c r="J24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K24" t="s">
         <v>169</v>
-      </c>
-      <c r="K24" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" t="s">
         <v>205</v>
       </c>
-      <c r="C25" t="s">
-        <v>206</v>
-      </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J25" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25" t="s">
         <v>171</v>
-      </c>
-      <c r="K25" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" t="s">
         <v>120</v>
       </c>
-      <c r="C26" t="s">
-        <v>121</v>
-      </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K26" t="s">
         <v>173</v>
-      </c>
-      <c r="K26" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J27" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" t="s">
         <v>175</v>
-      </c>
-      <c r="K27" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1619,227 +1619,227 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J28" t="s">
+        <v>176</v>
+      </c>
+      <c r="K28" t="s">
         <v>177</v>
-      </c>
-      <c r="K28" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" t="s">
         <v>98</v>
       </c>
-      <c r="G29" t="s">
-        <v>99</v>
-      </c>
       <c r="J29" t="s">
+        <v>178</v>
+      </c>
+      <c r="K29" t="s">
         <v>179</v>
-      </c>
-      <c r="K29" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F30" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" t="s">
         <v>165</v>
       </c>
-      <c r="G30" t="s">
-        <v>166</v>
-      </c>
       <c r="J30" t="s">
+        <v>180</v>
+      </c>
+      <c r="K30" t="s">
         <v>181</v>
-      </c>
-      <c r="K30" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F31" t="s">
+        <v>194</v>
+      </c>
+      <c r="G31" t="s">
         <v>195</v>
       </c>
-      <c r="G31" t="s">
-        <v>196</v>
-      </c>
       <c r="J31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
         <v>110</v>
       </c>
-      <c r="C32" t="s">
-        <v>111</v>
-      </c>
       <c r="F32" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" t="s">
         <v>197</v>
       </c>
-      <c r="G32" t="s">
-        <v>198</v>
-      </c>
       <c r="J32" t="s">
+        <v>184</v>
+      </c>
+      <c r="K32" t="s">
         <v>185</v>
-      </c>
-      <c r="K32" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" t="s">
         <v>112</v>
       </c>
-      <c r="C33" t="s">
-        <v>113</v>
-      </c>
       <c r="F33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J33" t="s">
+        <v>186</v>
+      </c>
+      <c r="K33" t="s">
         <v>187</v>
-      </c>
-      <c r="K33" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" t="s">
+        <v>199</v>
+      </c>
+      <c r="G34" t="s">
         <v>200</v>
       </c>
-      <c r="G34" t="s">
-        <v>201</v>
-      </c>
       <c r="J34" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" t="s">
         <v>189</v>
-      </c>
-      <c r="K34" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F35" t="s">
+        <v>201</v>
+      </c>
+      <c r="G35" t="s">
         <v>202</v>
       </c>
-      <c r="G35" t="s">
-        <v>203</v>
-      </c>
       <c r="J35" t="s">
+        <v>190</v>
+      </c>
+      <c r="K35" t="s">
         <v>191</v>
-      </c>
-      <c r="K35" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="C36" t="s">
-        <v>118</v>
-      </c>
       <c r="F36" t="s">
+        <v>207</v>
+      </c>
+      <c r="G36" t="s">
         <v>208</v>
       </c>
-      <c r="G36" t="s">
-        <v>209</v>
-      </c>
       <c r="J36" t="s">
+        <v>192</v>
+      </c>
+      <c r="K36" t="s">
         <v>193</v>
-      </c>
-      <c r="K36" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" t="s">
         <v>210</v>
-      </c>
-      <c r="C39" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40" t="s">
         <v>212</v>
-      </c>
-      <c r="C40" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>213</v>
+      </c>
+      <c r="C41" t="s">
         <v>214</v>
-      </c>
-      <c r="C41" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>